<commit_message>
ExceLoaderTest.xlsx for File Handlking
</commit_message>
<xml_diff>
--- a/ExceLoaderTest.xlsx
+++ b/ExceLoaderTest.xlsx
@@ -1,19 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Repos\XamlAml\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A14289F6-7AB1-40DE-804B-12C00EB870C1}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{060D543D-F81B-457B-BFAC-79CBC9D7B483}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3075" yWindow="0" windowWidth="25020" windowHeight="15600" xr2:uid="{92773C9E-5153-43F7-9340-6900A5F17D7A}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21240" activeTab="2" xr2:uid="{92773C9E-5153-43F7-9340-6900A5F17D7A}"/>
   </bookViews>
   <sheets>
-    <sheet name="User" sheetId="1" r:id="rId1"/>
+    <sheet name="CAD" sheetId="1" r:id="rId1"/>
+    <sheet name="CAD Strucure" sheetId="2" r:id="rId2"/>
+    <sheet name="CAD File" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,57 +36,60 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="17">
-  <si>
-    <t>login_name</t>
-  </si>
-  <si>
-    <t>email</t>
-  </si>
-  <si>
-    <t>password</t>
-  </si>
-  <si>
-    <t>user1</t>
-  </si>
-  <si>
-    <t>user2</t>
-  </si>
-  <si>
-    <t>user3</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="18">
   <si>
     <t>One</t>
   </si>
   <si>
-    <t>User</t>
-  </si>
-  <si>
-    <t>innovator</t>
-  </si>
-  <si>
-    <t>user1@innovator.com</t>
-  </si>
-  <si>
     <t>Two</t>
   </si>
   <si>
-    <t>Three</t>
-  </si>
-  <si>
-    <t>user2@innovator.com</t>
-  </si>
-  <si>
-    <t>user3@innovator.com</t>
-  </si>
-  <si>
-    <t>first_name</t>
-  </si>
-  <si>
-    <t>last_name</t>
-  </si>
-  <si>
-    <t>login_enabled</t>
+    <t>item_number</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">phsyical_file </t>
+  </si>
+  <si>
+    <t>owner(keyed_name)</t>
+  </si>
+  <si>
+    <t>001</t>
+  </si>
+  <si>
+    <t>002</t>
+  </si>
+  <si>
+    <t>native_file(filename)</t>
+  </si>
+  <si>
+    <t>config.xml</t>
+  </si>
+  <si>
+    <t>C:\Repos\XamlAml\config.xml</t>
+  </si>
+  <si>
+    <t>Innovator Admin</t>
+  </si>
+  <si>
+    <t>_blan2</t>
+  </si>
+  <si>
+    <t>_ignore</t>
+  </si>
+  <si>
+    <t>source_id(keyed_name)</t>
+  </si>
+  <si>
+    <t>related_id(keyed_name)</t>
+  </si>
+  <si>
+    <t>related_id(filename)</t>
+  </si>
+  <si>
+    <t>physical_file</t>
   </si>
 </sst>
 </file>
@@ -126,9 +131,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -443,102 +449,165 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D94D6732-BF9F-41CA-A9A3-21C1EE90ADB6}">
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:G4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="20.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11" customWidth="1"/>
+    <col min="5" max="5" width="28.5703125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="19.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" t="s">
         <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C1" t="s">
-        <v>15</v>
-      </c>
-      <c r="D1" t="s">
-        <v>1</v>
-      </c>
-      <c r="E1" t="s">
-        <v>2</v>
-      </c>
-      <c r="F1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C2" t="s">
-        <v>6</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>9</v>
       </c>
       <c r="E2" t="s">
-        <v>8</v>
-      </c>
-      <c r="F2">
+        <v>10</v>
+      </c>
+      <c r="F2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3" t="s">
+      <c r="D3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E3" t="s">
         <v>10</v>
       </c>
-      <c r="D3" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="E3" t="s">
-        <v>8</v>
-      </c>
-      <c r="F3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C4" t="s">
+      <c r="G3" t="s">
         <v>11</v>
       </c>
-      <c r="D4" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E4" t="s">
-        <v>8</v>
-      </c>
-      <c r="F4">
-        <v>1</v>
-      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D4" s="1"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B820F485-4C7E-482A-9680-243B8189903D}">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E16" sqref="E16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="22.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{20139360-1C4A-41C2-A327-0DEFDC9FD2D3}">
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="22.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>